<commit_message>
coreection html css validator mais il y a encore 4 erreur css que j ai pas compris et j ai ajouute defer au script js et changement bmp to png + leur allegement en terme de poids
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e7e8a701f7bea240/Bureau/apres_projet4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="11_91AA243AD46ACDB9E5A50D17A2E73107414BF062" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37A17861-C608-4151-8303-59CC5479A4E9}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="11_91AA243AD46ACDB9E5A50D17A2E73107414BF062" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17624D0D-664E-46B4-AEBB-C4CCAB1E0DDA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,9 +169,6 @@
     <t>img trop lourdes donc ralentissent le chargement de la page</t>
   </si>
   <si>
-    <t xml:space="preserve">augmenter le temps de chargement </t>
-  </si>
-  <si>
     <t>Augmentation du seo technique donc plus de chance d etre affiche plus haut</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>erreur basic style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dimunition le temps de chargement </t>
   </si>
 </sst>
 </file>
@@ -573,10 +573,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -782,8 +778,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1004,13 +1000,13 @@
         <v>48</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -1018,16 +1014,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -1035,16 +1031,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="E15" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="52.2" x14ac:dyDescent="0.3">
@@ -1052,16 +1048,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="E16" s="18" t="s">
         <v>61</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">

</xml_diff>